<commit_message>
Update VBT_Form_5th October 2021.xlsx
</commit_message>
<xml_diff>
--- a/Test cases/Nitish/VBT_Form_5th October 2021.xlsx
+++ b/Test cases/Nitish/VBT_Form_5th October 2021.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{62C4F565-2D9B-4B9F-BA68-42B8AB33893D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D6F576B-ED35-46E4-B2BA-48A8A0CD8F8F}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{62C4F565-2D9B-4B9F-BA68-42B8AB33893D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26547220-48FD-41C7-BA20-3AB396C78A0B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="780" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="780" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_KeywordFramework" sheetId="23" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4413" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4371" uniqueCount="314">
   <si>
     <t>GOTOURL</t>
   </si>
@@ -4221,22 +4221,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F96A65-3E86-40E7-8072-E8FF4573C506}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L65"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="17.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="51.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="8.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="23.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="4" width="17.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.5703125" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
-    <col min="11" max="16384" style="4" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="51.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="8.85546875" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6415,7 +6415,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F461771-B54A-4E13-A76D-2C0CF066DBA3}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -6423,23 +6423,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="25.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="17.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="25.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="15.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="4" width="15.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="14.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="17.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="4" width="18.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="3" width="14.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="4" width="15.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="4" width="14.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="3" width="14.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="4" width="26.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="4" width="24.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="3" width="25.42578125" collapsed="true"/>
-    <col min="17" max="16384" style="4" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14" style="3" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.140625" style="3" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="26.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="25.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="16384" width="8.85546875" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -6896,34 +6896,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="22.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="28.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="11.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="15" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="15" width="11.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="15" width="26.7109375" collapsed="true"/>
-    <col min="9" max="13" customWidth="true" style="15" width="12.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="4" width="28.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="4" width="19.140625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="4" width="12.42578125" collapsed="true"/>
-    <col min="17" max="19" customWidth="true" style="15" width="12.42578125" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="15" width="29.7109375" collapsed="true"/>
-    <col min="21" max="25" customWidth="true" style="15" width="12.42578125" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="4" width="29.85546875" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" style="4" width="12.5703125" collapsed="true"/>
-    <col min="29" max="31" customWidth="true" style="15" width="12.5703125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="15" width="29.28515625" collapsed="true"/>
-    <col min="33" max="37" customWidth="true" style="15" width="12.5703125" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="4" width="33.140625" collapsed="true"/>
-    <col min="39" max="39" customWidth="true" style="4" width="20.28515625" collapsed="true"/>
-    <col min="40" max="40" customWidth="true" style="4" width="11.28515625" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" style="4" width="15.42578125" collapsed="true"/>
-    <col min="42" max="43" style="4" width="8.85546875" collapsed="true"/>
-    <col min="44" max="49" style="4" width="8.85546875" collapsed="true"/>
-    <col min="50" max="16384" style="4" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="22.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.7109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="13" width="12.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="28.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.140625" style="4" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="17" max="19" width="12.42578125" style="15" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="29.7109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="21" max="25" width="12.42578125" style="15" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="29.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="16.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="29" max="31" width="12.5703125" style="15" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="29.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="37" width="12.5703125" style="15" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="33.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="20.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="15.42578125" style="4" customWidth="1" collapsed="1"/>
+    <col min="42" max="16384" width="8.85546875" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -17234,14 +17232,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="26.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="26.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="27.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="25.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="26.0" collapsed="true"/>
-    <col min="8" max="16384" style="4" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="8.85546875" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -17418,26 +17416,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA67551-36C0-4B16-863A-50AE8CC999D0}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="7.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="29.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="62" width="27.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="62" width="24.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="31" width="10.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="12.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="2" width="7" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.28515625" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.85546875" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.140625" style="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -17873,7 +17869,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -17958,16 +17954,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766D81E9-0BF1-46CE-819B-B4BF0FA64039}">
   <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+    <sheetView topLeftCell="A133" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="50.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="60" width="22.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" width="50.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" style="60" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20239,8 +20235,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -20461,8 +20457,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>